<commit_message>
add tables to doc
</commit_message>
<xml_diff>
--- a/Codes_Table.xlsx
+++ b/Codes_Table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CharlesKinze_xv2wdq5\Desktop\School\cv_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595B56BD-905F-4936-AA59-ABC0DB41A19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EC47C7-FA16-47D6-9E30-200C1948943E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{D9BACAE8-D834-43A6-BBC6-74EB2E1DA8DA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D9BACAE8-D834-43A6-BBC6-74EB2E1DA8DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -82,13 +83,25 @@
   </si>
   <si>
     <t>The level of prospective future work. Do the autheros lay out how to improve the solution? Are there obvious open ends to the research? A high score indicates a high propect.</t>
+  </si>
+  <si>
+    <t>TABLE I. TABLE TYPE STYLES</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE II. </t>
+  </si>
+  <si>
+    <t>TABLE II. Assessmetn Scores for Each Solution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +116,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -125,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -148,11 +173,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -174,6 +208,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E25DA1-57AF-48A0-98D3-F3FA9345760E}">
-  <dimension ref="H10:I31"/>
+  <dimension ref="H9:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,6 +555,12 @@
     <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
+    <row r="9" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
     <row r="10" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H10" s="5" t="s">
         <v>7</v>
@@ -609,7 +668,214 @@
       <c r="H31" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H9:I9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16FCF9B-C99E-436D-97D2-3F5B214C6CFD}">
+  <dimension ref="I7:P20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+    </row>
+    <row r="11" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I11" s="14">
+        <v>2</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+    </row>
+    <row r="12" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I12" s="13">
+        <v>3</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+    </row>
+    <row r="13" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I13" s="14">
+        <v>4</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+    </row>
+    <row r="14" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I14" s="13">
+        <v>5</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+    </row>
+    <row r="15" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I15" s="14">
+        <v>6</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+    </row>
+    <row r="16" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I16" s="13">
+        <v>7</v>
+      </c>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I17" s="14">
+        <v>8</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+    </row>
+    <row r="18" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I18" s="13">
+        <v>9</v>
+      </c>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+    </row>
+    <row r="19" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I19" s="14">
+        <v>10</v>
+      </c>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+    </row>
+    <row r="20" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I20" s="13">
+        <v>11</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I7:P7"/>
+    <mergeCell ref="I8:P8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>